<commit_message>
2022-12-08 JCS : renommage GED en Humathèque
</commit_message>
<xml_diff>
--- a/FulShortenedDueDateLetter/FulShortenedDueDateLetter-param-french.xlsx
+++ b/FulShortenedDueDateLetter/FulShortenedDueDateLetter-param-french.xlsx
@@ -5,21 +5,24 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.campus-condorcet.fr\Profils$\jérôme.chiavassa\Documents\Alma-Primo\Alma\Lettres\FulShortenedDueDateLetter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.campus-condorcet.fr\Profils$\jérôme.chiavassa\Documents\ALMA PRIMO\Alma\Lettres\FulShortenedDueDateLetter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="rowsForView" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rowsForView!$A$1:$F$10</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Activé</t>
   </si>
@@ -45,42 +48,42 @@
     <t>department</t>
   </si>
   <si>
-    <t>Grand équipement documentaire</t>
-  </si>
-  <si>
-    <t>L'équipe du Grand équipement documentaire</t>
+    <t>Humathèque</t>
+  </si>
+  <si>
+    <t>christine.aubree</t>
+  </si>
+  <si>
+    <t>Cc</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Aucun</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Bcc</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Shortened Due Date Letter</t>
+  </si>
+  <si>
+    <t>Date de retour modifiée pour le(s) document(s)</t>
   </si>
   <si>
     <t>jcs</t>
   </si>
   <si>
-    <t>Bcc</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Aucun</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Cc</t>
-  </si>
-  <si>
     <t>letterName</t>
   </si>
   <si>
-    <t>Shortened Due Date Letter</t>
-  </si>
-  <si>
-    <t>Date de retour modifiée pour le(s) document(s)</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
     <t>sincerely</t>
   </si>
   <si>
@@ -102,10 +105,7 @@
     <t>addressFrom</t>
   </si>
   <si>
-    <t>services.ged@campus-condorcet.fr</t>
-  </si>
-  <si>
-    <t>exl_impl</t>
+    <t>services.humatheque@campus-condorcet.fr</t>
   </si>
   <si>
     <t>due_back</t>
@@ -160,10 +160,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,211 +457,216 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2">
+        <v>44903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1">
-        <v>44204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>44903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1">
-        <v>43865</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>